<commit_message>
added data with dummy excel file
</commit_message>
<xml_diff>
--- a/dummy.xlsx
+++ b/dummy.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intel\Desktop\dummy_project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F232B9-5835-4624-8915-F2F86678B8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,34 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +362,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>